<commit_message>
add edge case scenarios
</commit_message>
<xml_diff>
--- a/FVPS.xlsx
+++ b/FVPS.xlsx
@@ -396,7 +396,7 @@
         <v>11500000</v>
       </c>
       <c r="D2" t="n">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="3">
@@ -412,7 +412,7 @@
         <v>10000000</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4">
@@ -428,7 +428,7 @@
         <v>7500000</v>
       </c>
       <c r="D4" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -460,7 +460,7 @@
         <v>11300000</v>
       </c>
       <c r="D6" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">

</xml_diff>